<commit_message>
Enviamos cambios en el archivo perfiles.xlsx
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -2875,7 +2875,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3147,7 +3147,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="22" t="n">

</xml_diff>

<commit_message>
Trabajo al 21 de julio de 2017
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -2875,7 +2875,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="22" t="n">
@@ -3178,7 +3178,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="22" t="n">
@@ -3201,7 +3201,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="22" t="n">
@@ -3221,7 +3221,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="22" t="n">
@@ -3235,7 +3235,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="22" t="n">

</xml_diff>

<commit_message>
Envío del trabajo hasta el 24 de julio
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="97">
   <si>
     <t xml:space="preserve">Perfil</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">Producción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relacion Proveedor – Producto</t>
   </si>
 </sst>
 </file>
@@ -2872,10 +2875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3039,7 +3042,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="22" t="n">
@@ -3059,7 +3062,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="22" t="n">
@@ -3365,80 +3368,88 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B27" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="22" t="n">
+      <c r="C27" s="22" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="23" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="22" t="n">
+      <c r="C28" s="22" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B30" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="22" t="n">
+      <c r="C30" s="22" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="23" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="22" t="n">
+      <c r="C31" s="22" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B33" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="22" t="n">
+      <c r="C33" s="22" t="n">
         <v>30</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="22" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="22" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="22" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="22" t="n">
+      <c r="C36" s="22" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Envio el trabajo de ayer
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Perfiles" sheetId="1" state="visible" r:id="rId2"/>
@@ -724,12 +724,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.4453441295547"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
@@ -2878,25 +2878,25 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.3846153846154"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.5991902834008"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="22" t="n">

</xml_diff>

<commit_message>
Enviando el trabajo hasta el 31 de julio
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Perfiles" sheetId="1" state="visible" r:id="rId2"/>
@@ -724,12 +724,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.0890688259109"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
@@ -2875,28 +2875,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.8137651821862"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
@@ -3449,7 +3449,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Arreglando un bug en la creación de menús
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -2889,8 +2889,8 @@
   </sheetPr>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>